<commit_message>
create * & +
</commit_message>
<xml_diff>
--- a/錯誤代碼.xlsx
+++ b/錯誤代碼.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0obriano0\Documents\GitHub\Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{26316C4C-A8CE-40E6-BF8E-B72E6E40C50D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{83957484-BD78-47F9-A64F-891AF5902C9B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{38F7FC1F-128D-40D6-8E7C-E978A0B78D5E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,6 +40,10 @@
   </si>
   <si>
     <t>括弧前面不是符號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+的處裡出現問題</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -129,7 +133,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -140,6 +144,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC6EEA9-5875-49A7-A5C7-114E69ABF832}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -492,6 +499,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add more message show
</commit_message>
<xml_diff>
--- a/錯誤代碼.xlsx
+++ b/錯誤代碼.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0obriano0\Documents\GitHub\Calculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2034A5E9-86C9-4855-877E-5DE05B4DEF69}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF60B8B-9E6C-401F-8529-57DC7D49966F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" activeTab="1" xr2:uid="{38F7FC1F-128D-40D6-8E7C-E978A0B78D5E}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{38F7FC1F-128D-40D6-8E7C-E978A0B78D5E}"/>
   </bookViews>
   <sheets>
     <sheet name="錯誤代碼" sheetId="1" r:id="rId1"/>
     <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,12 +64,27 @@
   </si>
   <si>
     <t>3+1*(5+8-5*(3-2))</t>
+  </si>
+  <si>
+    <t>(((sin(0.5*(3+1*(5+8-5*(3-2))))*6*(3+1*(5+8-5*(3-2))))+0.5*(3+1*(5+8-5))*10!)+(0.5*(3+1*(5+8-5)))*4+3+1*(5+8-5*(3-2)))/70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(((sin(0.5*(3+1*(5+8-5*(3-2))))*6*(3+1*(5+8-5*(3-2))))+0.5*(3+1*(5+8-5))*10!)+(0.5*(3+1*(5+8-5)))*4+3+1*(5+8-5*(3-2)))/70+(((sin(0.5*(3+1*(5+8-5*(3-2))))*6*(3+1*(5+8-5*(3-2))))+0.5*(3+1*(5+8-5))*10!)+(0.5*(3+1*(5+8-5)))*4+3+1*(5+8-5*(3-2)))/70/90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(((sin(0.5*(3+1*(5+8-5*(3-2))))*6*(3+1*(5+8-5*(3-2))))+0.5*(3+1*(5+8-5))*10!)+(0.5*(3+1*(5+8-5)))*4+3+1*(5+8-5*(3-2)))/70+(((sin(0.5*(3+1*(5+8-5*(3-2))))*6*(3+1*(5+8-5*(3-2))))+0.5*(3+1*(5+8-5))*10!)+(0.5*(3+1*(5+8-5)))*4+3+1*(5+8-5*(3-2)))/70/90-(((sin(0.5*(3+1*(5+8-5*(3-2))))*6*(3+1*(5+8-5*(3-2))))+0.5*(3+1*(5+8-5))*10!)+(0.5*(3+1*(5+8-5)))*4+3+1*(5+8-5*(3-2)))/70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.0000_);[Red]\(0.0000\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -152,7 +167,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -167,6 +182,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,22 +553,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3B6F87-371C-41D0-885D-023AC463B1C0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="118.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -558,7 +577,7 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>5.5</v>
       </c>
     </row>
@@ -566,7 +585,7 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>5.5</v>
       </c>
     </row>
@@ -574,8 +593,32 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
+        <v>285119.80620499997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
+        <v>288287.80405199999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3167.9978470000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>